<commit_message>
Change Icon, changed calculator stuff
</commit_message>
<xml_diff>
--- a/gpa_calculator/gpa_data.xlsx
+++ b/gpa_calculator/gpa_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,23 +476,48 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Semester 1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>4.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Semester 2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Englishj</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C4" t="n">
         <v>3</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>3.00</t>
         </is>

</xml_diff>

<commit_message>
Centered GPA calculator main page
</commit_message>
<xml_diff>
--- a/gpa_calculator/gpa_data.xlsx
+++ b/gpa_calculator/gpa_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Math</t>
+          <t>Calculus</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -469,7 +469,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>4.00</t>
+          <t>3.88</t>
         </is>
       </c>
     </row>
@@ -481,7 +481,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>English</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -494,19 +494,19 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>4.00</t>
+          <t>3.88</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Semester 2</t>
+          <t>Semester 1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Englishj</t>
+          <t>PROBLEM SOLVING AND PROGRAMMING</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -514,12 +514,87 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>A-</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3.88</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Semester 2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	FUNDAMENTALS OF COMPUTER NETWORKS</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>3.00</t>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>3.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Semester 2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PROBABILITY AND STATISTICS</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>B+</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>3.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Semester 2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>COMPUTER ARCHITECTURE</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>3.10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GPA Calculator Maybe completed
</commit_message>
<xml_diff>
--- a/gpa_calculator/gpa_data.xlsx
+++ b/gpa_calculator/gpa_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GPA Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="GPA Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,6 +448,431 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Semester 1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Database Development</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2.6995</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Semester 1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>English for Tertiary Studies</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>B+</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2.6995</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Semester 1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Problem Solving and Programming</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>B+</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2.6995</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Semester 1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Introduction to Cybersecurity</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>B-</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2.6995</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Semester 1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>System Analysis and Design</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2.6995</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Semester 1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Integrity and Anti-Corruption</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2.6995</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Semester 1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Calculus and Algebra</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2.6995</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Semester 2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Fundamentals of Computer Network</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>B+</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2.1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Semester 2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Probability and Statistics</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>C+</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2.1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Semester 2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Computer Architecture</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>C+</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2.1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Semester 2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Calculus and Algebra</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2.1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Semester 3</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Object-Oriented Programming</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>B+</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>3.4665</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Semester 3</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Introduction to Interface Design</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>A-</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>3.4665</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Semester 3</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Academic English</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>A-</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>3.4665</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Semester 3</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Web-based Integration Systems</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>3.4665</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Semester 3</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Discrete Mathematics</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>3.4665</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Semester 3</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Penghayatan Etika dan Peradaban</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>B+</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>3.4665</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>